<commit_message>
KFP Support files added & updated
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/KFP/ALL_PAGES/END_TO_END/TC15_Verify_MyaccountSection_for_all_Usertype.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/KFP/ALL_PAGES/END_TO_END/TC15_Verify_MyaccountSection_for_all_Usertype.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Actual_testcases\Kaman\ECTEST\KFP\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED65E395-BA65-431D-B745-561FC8EE8CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3B17D9-A075-4404-AF0F-F741456C3C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2216,6 +2216,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -2412,12 +2418,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
@@ -2427,6 +2427,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2443,21 +2460,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>